<commit_message>
All the stuff from costs is updated
</commit_message>
<xml_diff>
--- a/Cost/Agrisos/Cost_List.xlsx
+++ b/Cost/Agrisos/Cost_List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Total Recibido</t>
   </si>
@@ -33,13 +33,22 @@
     <t>Left:</t>
   </si>
   <si>
-    <t>Vaina</t>
-  </si>
-  <si>
     <t>Precio_U</t>
   </si>
   <si>
     <t>P_total</t>
+  </si>
+  <si>
+    <t>APM 2.6</t>
+  </si>
+  <si>
+    <t>Helicopter</t>
+  </si>
+  <si>
+    <t>Flatmaps</t>
+  </si>
+  <si>
+    <t>RD900 radio</t>
   </si>
 </sst>
 </file>
@@ -77,10 +86,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,14 +403,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
       <c r="C1">
         <v>5000</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>42279</v>
       </c>
     </row>
@@ -413,17 +422,17 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="2"/>
       <c r="C5">
         <v>1</v>
       </c>
@@ -436,190 +445,217 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>239.98</v>
+      </c>
       <c r="E6">
         <f t="shared" ref="E6:E26" si="0">D6*C6</f>
-        <v>0</v>
+        <v>479.96</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>335.41</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>335.41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>164.5</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>164.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>203.28</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>203.28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="E13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="E14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="E16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="E17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="E18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
       <c r="E19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
       <c r="E20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="E21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
       <c r="E22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
       <c r="E23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="E24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
       <c r="E25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
       <c r="E26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="2"/>
       <c r="D28">
         <f>C1-SUM(E5:E26)</f>
-        <v>3500</v>
+        <v>2316.85</v>
       </c>
     </row>
   </sheetData>
@@ -631,11 +667,6 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -643,12 +674,17 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lastest changes in budget
</commit_message>
<xml_diff>
--- a/Cost/Agrisos/Cost_List.xlsx
+++ b/Cost/Agrisos/Cost_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="9030"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Total Recibido</t>
   </si>
@@ -51,9 +51,6 @@
     <t>RD900 radio</t>
   </si>
   <si>
-    <t>Bought</t>
-  </si>
-  <si>
     <t>Status (Bought,Shipped,Obtained)</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Delivered</t>
+  </si>
+  <si>
+    <t>SpektrumRadio+TelemetryPower</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,19 +505,19 @@
         <v>6</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
         <v>19</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -536,13 +536,13 @@
         <v>1545</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N5" s="1">
         <v>42053</v>
@@ -564,7 +564,7 @@
         <v>479.96</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -583,13 +583,13 @@
         <v>335.41</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="J7" s="4">
         <v>780198136296</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" s="1">
         <v>42051</v>
@@ -611,7 +611,7 @@
         <v>164.5</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -631,13 +631,13 @@
         <v>209.38</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="J9" s="3">
         <v>5881663535</v>
       </c>
       <c r="M9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N9" s="1">
         <v>42051</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10">
@@ -659,13 +659,13 @@
         <v>314.44</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N10" s="1">
         <v>42053</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11">
@@ -687,12 +687,12 @@
         <v>69.989999999999995</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12">
@@ -706,15 +706,26 @@
         <v>17.88</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B13" s="5"/>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>270.83</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>270.83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -832,18 +843,18 @@
       <c r="B28" s="5"/>
       <c r="D28">
         <f>C1-SUM(E5:E26)</f>
-        <v>1863.44</v>
+        <v>1592.6100000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -856,13 +867,13 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J7" r:id="rId1" display="http://www.fedex.com/Tracking?language=english&amp;cntry_code=us&amp;tracknumbers=780198136296"/>

</xml_diff>